<commit_message>
Added PAD Advanced Settings Screen
</commit_message>
<xml_diff>
--- a/Documentation/Navigation_FEB1721.xlsx
+++ b/Documentation/Navigation_FEB1721.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\asl\ASL4321_Project\ASL4321_Display_Demo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318CA1B8-5667-456B-AE15-21CA49EE4839}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA5B27A-1858-418B-A7AE-DF9099C2F4AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -759,9 +759,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -778,6 +775,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1296,50 +1296,6 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>22201</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="37" name="Picture 36">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000025000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12230100" y="4191000"/>
-          <a:ext cx="2460601" cy="1400175"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
@@ -1430,7 +1386,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1474,7 +1430,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1790,7 +1746,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1834,7 +1790,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1878,7 +1834,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1985,7 +1941,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2109,50 +2065,6 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>68</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>18317</xdr:colOff>
-      <xdr:row>76</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="51" name="Picture 50">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000033000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="9182100" y="11229975"/>
-          <a:ext cx="2456717" cy="1400175"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
@@ -2243,7 +2155,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2487,7 +2399,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2807,7 +2719,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2851,7 +2763,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3234,7 +3146,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3243,50 +3155,6 @@
         <a:xfrm>
           <a:off x="9182100" y="11049000"/>
           <a:ext cx="2447925" cy="1392257"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>1605</xdr:colOff>
-      <xdr:row>66</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="70" name="Picture 69">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000046000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="12839700" y="11239500"/>
-          <a:ext cx="2440005" cy="1390650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3356,6 +3224,370 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>88421</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C6ADB1C-EF0C-4186-AA30-7363D5084104}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12344400" y="4200526"/>
+          <a:ext cx="2457449" cy="1421920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>552451</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>564365</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1F35990D-514A-48C3-B609-0547E8F274B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16440151" y="4200526"/>
+          <a:ext cx="2450314" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>141722</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>116700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="Right Arrow 40">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{079C9AB2-D27F-47B5-8E66-37A50EF9CE2C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13591022" y="5079225"/>
+          <a:ext cx="2811028" cy="311925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightArrow">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 53137"/>
+            <a:gd name="adj2" fmla="val 74489"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>400049</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="73" name="Rectangular Callout 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB1EFAEC-F9F9-4C92-9FAA-B5B5E32F201A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19592924" y="4848225"/>
+          <a:ext cx="2181225" cy="1714500"/>
+        </a:xfrm>
+        <a:prstGeom prst="wedgeRectCallout">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val -111851"/>
+            <a:gd name="adj2" fmla="val -45012"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>This is a</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> scrolling list.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>It has....</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>- FORWARD, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>LEFT. RIGHT, </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>REVERSE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>- NEXT</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> FUNCTION</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- NEXT PROFILE</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>- SEATING options</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Anything that we want to control with a long press.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>26566</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{585D3EA6-2763-4DF3-B9EC-09FC74517CE2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12849225" y="11249026"/>
+          <a:ext cx="2455441" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>59462</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA85A8E4-2DF9-4501-8B99-8C1BAFDBDB59}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9182100" y="13144500"/>
+          <a:ext cx="2447925" cy="1392962"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -5019,10 +5251,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="26"/>
+      <c r="C1" s="32"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5079,18 +5311,18 @@
     </row>
     <row r="3" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="28"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -5139,22 +5371,22 @@
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="29"/>
-      <c r="D5" s="29" t="s">
+      <c r="C5" s="28"/>
+      <c r="D5" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29" t="s">
+      <c r="E5" s="28"/>
+      <c r="F5" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="29"/>
-      <c r="H5" s="29" t="s">
+      <c r="G5" s="28"/>
+      <c r="H5" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="29"/>
+      <c r="I5" s="28"/>
       <c r="J5" s="1" t="s">
         <v>5</v>
       </c>
@@ -5227,28 +5459,28 @@
     </row>
     <row r="7" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="H7" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="30" t="s">
+      <c r="I7" s="29" t="s">
         <v>11</v>
       </c>
       <c r="J7" s="5" t="s">
@@ -5278,14 +5510,14 @@
     </row>
     <row r="8" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="I8" s="31"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
       <c r="J8" s="5" t="s">
         <v>16</v>
       </c>
@@ -5311,14 +5543,14 @@
     </row>
     <row r="9" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="32"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="32"/>
-      <c r="E9" s="32"/>
-      <c r="F9" s="32"/>
-      <c r="G9" s="32"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="32"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
       <c r="J9" s="5" t="s">
         <v>18</v>
       </c>
@@ -5373,18 +5605,18 @@
     </row>
     <row r="11" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="27"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -5433,22 +5665,22 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29" t="s">
+      <c r="C13" s="28"/>
+      <c r="D13" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29" t="s">
+      <c r="E13" s="28"/>
+      <c r="F13" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29" t="s">
+      <c r="G13" s="28"/>
+      <c r="H13" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="29"/>
+      <c r="I13" s="28"/>
       <c r="J13" s="1" t="s">
         <v>5</v>
       </c>
@@ -5521,28 +5753,28 @@
     </row>
     <row r="15" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="30" t="s">
+      <c r="G15" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="30" t="s">
+      <c r="H15" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="30" t="s">
+      <c r="I15" s="29" t="s">
         <v>22</v>
       </c>
       <c r="J15" s="5" t="s">
@@ -5572,14 +5804,14 @@
     </row>
     <row r="16" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="31"/>
-      <c r="F16" s="31"/>
-      <c r="G16" s="31"/>
-      <c r="H16" s="31"/>
-      <c r="I16" s="31"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
       <c r="J16" s="5" t="s">
         <v>16</v>
       </c>
@@ -5607,14 +5839,14 @@
     </row>
     <row r="17" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
-      <c r="F17" s="31"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
       <c r="J17" s="5" t="s">
         <v>25</v>
       </c>
@@ -5642,14 +5874,14 @@
     </row>
     <row r="18" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
-      <c r="G18" s="31"/>
-      <c r="H18" s="31"/>
-      <c r="I18" s="31"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
       <c r="J18" s="5" t="s">
         <v>27</v>
       </c>
@@ -5677,14 +5909,14 @@
     </row>
     <row r="19" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
+      <c r="I19" s="31"/>
       <c r="J19" s="5" t="s">
         <v>25</v>
       </c>
@@ -5741,18 +5973,18 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -5801,22 +6033,22 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29" t="s">
+      <c r="C23" s="28"/>
+      <c r="D23" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29" t="s">
+      <c r="E23" s="28"/>
+      <c r="F23" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29" t="s">
+      <c r="G23" s="28"/>
+      <c r="H23" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="29"/>
+      <c r="I23" s="28"/>
       <c r="J23" s="1" t="s">
         <v>5</v>
       </c>
@@ -6231,18 +6463,18 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="28"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
-      <c r="K35" s="28"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="27"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
+      <c r="J35" s="27"/>
+      <c r="K35" s="27"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
@@ -6291,22 +6523,22 @@
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29" t="s">
+      <c r="C37" s="28"/>
+      <c r="D37" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29" t="s">
+      <c r="E37" s="28"/>
+      <c r="F37" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G37" s="29"/>
-      <c r="H37" s="29" t="s">
+      <c r="G37" s="28"/>
+      <c r="H37" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I37" s="29"/>
+      <c r="I37" s="28"/>
       <c r="J37" s="1" t="s">
         <v>5</v>
       </c>
@@ -6379,28 +6611,28 @@
     </row>
     <row r="39" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="30" t="s">
+      <c r="C39" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D39" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="30" t="s">
+      <c r="E39" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="F39" s="30" t="s">
+      <c r="F39" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="30" t="s">
+      <c r="G39" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="H39" s="30" t="s">
+      <c r="H39" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="I39" s="30" t="s">
+      <c r="I39" s="29" t="s">
         <v>47</v>
       </c>
       <c r="J39" s="8" t="s">
@@ -6428,14 +6660,14 @@
     </row>
     <row r="40" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-      <c r="I40" s="31"/>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
       <c r="J40" s="8" t="s">
         <v>27</v>
       </c>
@@ -6463,14 +6695,14 @@
     </row>
     <row r="41" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="32"/>
-      <c r="I41" s="32"/>
+      <c r="B41" s="31"/>
+      <c r="C41" s="31"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
+      <c r="I41" s="31"/>
       <c r="J41" s="8" t="s">
         <v>45</v>
       </c>
@@ -6496,18 +6728,18 @@
     </row>
     <row r="43" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="28"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="28"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="28"/>
-      <c r="H43" s="28"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="28"/>
-      <c r="K43" s="28"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="27"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="27"/>
+      <c r="G43" s="27"/>
+      <c r="H43" s="27"/>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
@@ -6556,22 +6788,22 @@
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="B45" s="29" t="s">
+      <c r="B45" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29" t="s">
+      <c r="C45" s="28"/>
+      <c r="D45" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="29"/>
-      <c r="F45" s="29" t="s">
+      <c r="E45" s="28"/>
+      <c r="F45" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29" t="s">
+      <c r="G45" s="28"/>
+      <c r="H45" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I45" s="29"/>
+      <c r="I45" s="28"/>
       <c r="J45" s="1" t="s">
         <v>5</v>
       </c>
@@ -6712,18 +6944,18 @@
     </row>
     <row r="50" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="27" t="s">
+      <c r="B50" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
-      <c r="F50" s="28"/>
-      <c r="G50" s="28"/>
-      <c r="H50" s="28"/>
-      <c r="I50" s="28"/>
-      <c r="J50" s="28"/>
-      <c r="K50" s="28"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="27"/>
+      <c r="K50" s="27"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
@@ -6772,22 +7004,22 @@
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="B52" s="29" t="s">
+      <c r="B52" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C52" s="29"/>
-      <c r="D52" s="29" t="s">
+      <c r="C52" s="28"/>
+      <c r="D52" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E52" s="29"/>
-      <c r="F52" s="29" t="s">
+      <c r="E52" s="28"/>
+      <c r="F52" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G52" s="29"/>
-      <c r="H52" s="29" t="s">
+      <c r="G52" s="28"/>
+      <c r="H52" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I52" s="29"/>
+      <c r="I52" s="28"/>
       <c r="J52" s="1" t="s">
         <v>5</v>
       </c>
@@ -6925,18 +7157,18 @@
     </row>
     <row r="57" spans="1:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="B57" s="27" t="s">
+      <c r="B57" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="C57" s="28"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="28"/>
-      <c r="F57" s="28"/>
-      <c r="G57" s="28"/>
-      <c r="H57" s="28"/>
-      <c r="I57" s="28"/>
-      <c r="J57" s="28"/>
-      <c r="K57" s="28"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="27"/>
+      <c r="H57" s="27"/>
+      <c r="I57" s="27"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="27"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
@@ -6956,22 +7188,22 @@
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-      <c r="B58" s="29" t="s">
+      <c r="B58" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="29"/>
-      <c r="D58" s="29" t="s">
+      <c r="C58" s="28"/>
+      <c r="D58" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E58" s="29"/>
-      <c r="F58" s="29" t="s">
+      <c r="E58" s="28"/>
+      <c r="F58" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="G58" s="29"/>
-      <c r="H58" s="29" t="s">
+      <c r="G58" s="28"/>
+      <c r="H58" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="I58" s="29"/>
+      <c r="I58" s="28"/>
       <c r="J58" s="1" t="s">
         <v>5</v>
       </c>
@@ -7141,30 +7373,50 @@
     </row>
   </sheetData>
   <mergeCells count="84">
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="H60:H61"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
-    <mergeCell ref="B57:K57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H15:H19"/>
-    <mergeCell ref="I15:I19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="G54:G55"/>
+    <mergeCell ref="H54:H55"/>
+    <mergeCell ref="I54:I55"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B50:K50"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="F52:G52"/>
+    <mergeCell ref="H52:I52"/>
+    <mergeCell ref="B54:B55"/>
+    <mergeCell ref="C54:C55"/>
+    <mergeCell ref="D54:D55"/>
+    <mergeCell ref="E54:E55"/>
+    <mergeCell ref="F54:F55"/>
+    <mergeCell ref="I39:I41"/>
+    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="H39:H41"/>
+    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="G25:G33"/>
+    <mergeCell ref="H25:H33"/>
+    <mergeCell ref="I25:I33"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B25:B33"/>
+    <mergeCell ref="C25:C33"/>
+    <mergeCell ref="D25:D33"/>
+    <mergeCell ref="E25:E33"/>
+    <mergeCell ref="F25:F33"/>
     <mergeCell ref="B3:K3"/>
     <mergeCell ref="B11:K11"/>
     <mergeCell ref="B21:K21"/>
@@ -7181,50 +7433,30 @@
     <mergeCell ref="H7:H9"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="G25:G33"/>
-    <mergeCell ref="H25:H33"/>
-    <mergeCell ref="I25:I33"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B25:B33"/>
-    <mergeCell ref="C25:C33"/>
-    <mergeCell ref="D25:D33"/>
-    <mergeCell ref="E25:E33"/>
-    <mergeCell ref="F25:F33"/>
-    <mergeCell ref="B35:K35"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="H39:H41"/>
-    <mergeCell ref="G54:G55"/>
-    <mergeCell ref="H54:H55"/>
-    <mergeCell ref="I54:I55"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="B50:K50"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="F52:G52"/>
-    <mergeCell ref="H52:I52"/>
-    <mergeCell ref="B54:B55"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="D54:D55"/>
-    <mergeCell ref="E54:E55"/>
-    <mergeCell ref="F54:F55"/>
-    <mergeCell ref="I39:I41"/>
-    <mergeCell ref="B43:K43"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="I15:I19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="B57:K57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="H60:H61"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7236,8 +7468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C3:W48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X61" sqref="X61"/>
+    <sheetView tabSelected="1" topLeftCell="E47" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M70" sqref="M70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added Single and Dual switch processing, but not done
</commit_message>
<xml_diff>
--- a/Documentation/Navigation_FEB1721.xlsx
+++ b/Documentation/Navigation_FEB1721.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\asl\ASL4321_Project\ASL4321_Display_Demo\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA5B27A-1858-418B-A7AE-DF9099C2F4AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8039C274-A9A3-4B48-B39F-AD67439FC6A2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26565" yWindow="510" windowWidth="24105" windowHeight="14655" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings and Navigation" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="157">
   <si>
     <t>LEFT PAD</t>
   </si>
@@ -540,12 +540,30 @@
   <si>
     <t>Quadrant</t>
   </si>
+  <si>
+    <t>Single Switch selected.</t>
+  </si>
+  <si>
+    <t>Two-Switch selected.</t>
+  </si>
+  <si>
+    <t>SINGLE and TWO-SWITCH opreration.</t>
+  </si>
+  <si>
+    <t>ORANGE circle highlights scanned item.</t>
+  </si>
+  <si>
+    <t>GREEN circles highlight active feature and operate using the switch.</t>
+  </si>
+  <si>
+    <t>When the "cross" is selected, as depicted below, the system activates the feature (short press) or advances to the next feature (long press).</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -597,6 +615,13 @@
     </font>
     <font>
       <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -690,7 +715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -759,6 +784,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -777,9 +805,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3590,6 +3616,94 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>608047</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F64264D-E923-45EF-B37B-8D747EE59FAB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17106900" y="962025"/>
+          <a:ext cx="1827247" cy="1057275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>112807</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4C51E05-E296-4CE9-900F-DC8F9DDDD279}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19535775" y="962026"/>
+          <a:ext cx="1838325" cy="1065306"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4969,6 +5083,138 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>22167</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72B6A434-F87D-4874-8EDD-77B6592ABF32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="19050001"/>
+          <a:ext cx="2460567" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>100</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>17041</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{167AB12E-8722-4C06-BEF0-5552976A7F32}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4267200" y="19050001"/>
+          <a:ext cx="2455441" cy="1409700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>80624</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CAF675EA-BCEB-472B-8288-B1A2E8880FBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="21336000"/>
+          <a:ext cx="2466975" cy="1414124"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5251,10 +5497,10 @@
   <sheetData>
     <row r="1" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C1" s="32"/>
+      <c r="C1" s="26"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -5311,18 +5557,18 @@
     </row>
     <row r="3" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -5371,22 +5617,22 @@
     </row>
     <row r="5" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28" t="s">
+      <c r="C5" s="29"/>
+      <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="28" t="s">
+      <c r="E5" s="29"/>
+      <c r="F5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28" t="s">
+      <c r="G5" s="29"/>
+      <c r="H5" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="28"/>
+      <c r="I5" s="29"/>
       <c r="J5" s="1" t="s">
         <v>5</v>
       </c>
@@ -5459,28 +5705,28 @@
     </row>
     <row r="7" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="29" t="s">
+      <c r="H7" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="I7" s="29" t="s">
+      <c r="I7" s="30" t="s">
         <v>11</v>
       </c>
       <c r="J7" s="5" t="s">
@@ -5510,14 +5756,14 @@
     </row>
     <row r="8" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="30"/>
-      <c r="I8" s="30"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
       <c r="J8" s="5" t="s">
         <v>16</v>
       </c>
@@ -5543,14 +5789,14 @@
     </row>
     <row r="9" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="31"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
       <c r="J9" s="5" t="s">
         <v>18</v>
       </c>
@@ -5605,18 +5851,18 @@
     </row>
     <row r="11" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -5665,22 +5911,22 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28" t="s">
+      <c r="C13" s="29"/>
+      <c r="D13" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28" t="s">
+      <c r="E13" s="29"/>
+      <c r="F13" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="28"/>
-      <c r="H13" s="28" t="s">
+      <c r="G13" s="29"/>
+      <c r="H13" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="28"/>
+      <c r="I13" s="29"/>
       <c r="J13" s="1" t="s">
         <v>5</v>
       </c>
@@ -5753,28 +5999,28 @@
     </row>
     <row r="15" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="29" t="s">
+      <c r="D15" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="29" t="s">
+      <c r="E15" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="29" t="s">
+      <c r="G15" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H15" s="29" t="s">
+      <c r="H15" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="I15" s="29" t="s">
+      <c r="I15" s="30" t="s">
         <v>22</v>
       </c>
       <c r="J15" s="5" t="s">
@@ -5804,14 +6050,14 @@
     </row>
     <row r="16" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="30"/>
-      <c r="E16" s="30"/>
-      <c r="F16" s="30"/>
-      <c r="G16" s="30"/>
-      <c r="H16" s="30"/>
-      <c r="I16" s="30"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
+      <c r="H16" s="31"/>
+      <c r="I16" s="31"/>
       <c r="J16" s="5" t="s">
         <v>16</v>
       </c>
@@ -5839,14 +6085,14 @@
     </row>
     <row r="17" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
-      <c r="I17" s="30"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
+      <c r="H17" s="31"/>
+      <c r="I17" s="31"/>
       <c r="J17" s="5" t="s">
         <v>25</v>
       </c>
@@ -5874,14 +6120,14 @@
     </row>
     <row r="18" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="30"/>
-      <c r="D18" s="30"/>
-      <c r="E18" s="30"/>
-      <c r="F18" s="30"/>
-      <c r="G18" s="30"/>
-      <c r="H18" s="30"/>
-      <c r="I18" s="30"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
       <c r="J18" s="5" t="s">
         <v>27</v>
       </c>
@@ -5909,14 +6155,14 @@
     </row>
     <row r="19" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="31"/>
-      <c r="I19" s="31"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
       <c r="J19" s="5" t="s">
         <v>25</v>
       </c>
@@ -5973,18 +6219,18 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
@@ -6033,22 +6279,22 @@
     </row>
     <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28" t="s">
+      <c r="C23" s="29"/>
+      <c r="D23" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28" t="s">
+      <c r="E23" s="29"/>
+      <c r="F23" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28" t="s">
+      <c r="G23" s="29"/>
+      <c r="H23" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="I23" s="28"/>
+      <c r="I23" s="29"/>
       <c r="J23" s="1" t="s">
         <v>5</v>
       </c>
@@ -6463,18 +6709,18 @@
     </row>
     <row r="35" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="26" t="s">
+      <c r="B35" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="27"/>
-      <c r="E35" s="27"/>
-      <c r="F35" s="27"/>
-      <c r="G35" s="27"/>
-      <c r="H35" s="27"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="28"/>
+      <c r="H35" s="28"/>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
@@ -6523,22 +6769,22 @@
     </row>
     <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C37" s="28"/>
-      <c r="D37" s="28" t="s">
+      <c r="C37" s="29"/>
+      <c r="D37" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E37" s="28"/>
-      <c r="F37" s="28" t="s">
+      <c r="E37" s="29"/>
+      <c r="F37" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G37" s="28"/>
-      <c r="H37" s="28" t="s">
+      <c r="G37" s="29"/>
+      <c r="H37" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="I37" s="28"/>
+      <c r="I37" s="29"/>
       <c r="J37" s="1" t="s">
         <v>5</v>
       </c>
@@ -6611,28 +6857,28 @@
     </row>
     <row r="39" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="29" t="s">
+      <c r="C39" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="D39" s="29" t="s">
+      <c r="D39" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="E39" s="29" t="s">
+      <c r="E39" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F39" s="29" t="s">
+      <c r="F39" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="G39" s="29" t="s">
+      <c r="G39" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H39" s="29" t="s">
+      <c r="H39" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="I39" s="29" t="s">
+      <c r="I39" s="30" t="s">
         <v>47</v>
       </c>
       <c r="J39" s="8" t="s">
@@ -6660,14 +6906,14 @@
     </row>
     <row r="40" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
+      <c r="I40" s="31"/>
       <c r="J40" s="8" t="s">
         <v>27</v>
       </c>
@@ -6695,14 +6941,14 @@
     </row>
     <row r="41" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
-      <c r="I41" s="31"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="32"/>
+      <c r="F41" s="32"/>
+      <c r="G41" s="32"/>
+      <c r="H41" s="32"/>
+      <c r="I41" s="32"/>
       <c r="J41" s="8" t="s">
         <v>45</v>
       </c>
@@ -6728,18 +6974,18 @@
     </row>
     <row r="43" spans="1:27" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="27" t="s">
         <v>52</v>
       </c>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="28"/>
+      <c r="I43" s="28"/>
+      <c r="J43" s="28"/>
+      <c r="K43" s="28"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
       <c r="N43" s="1"/>
@@ -6788,22 +7034,22 @@
     </row>
     <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="B45" s="28" t="s">
+      <c r="B45" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28" t="s">
+      <c r="C45" s="29"/>
+      <c r="D45" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E45" s="28"/>
-      <c r="F45" s="28" t="s">
+      <c r="E45" s="29"/>
+      <c r="F45" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G45" s="28"/>
-      <c r="H45" s="28" t="s">
+      <c r="G45" s="29"/>
+      <c r="H45" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="I45" s="28"/>
+      <c r="I45" s="29"/>
       <c r="J45" s="1" t="s">
         <v>5</v>
       </c>
@@ -6944,18 +7190,18 @@
     </row>
     <row r="50" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
-      <c r="J50" s="27"/>
-      <c r="K50" s="27"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="28"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28"/>
+      <c r="G50" s="28"/>
+      <c r="H50" s="28"/>
+      <c r="I50" s="28"/>
+      <c r="J50" s="28"/>
+      <c r="K50" s="28"/>
       <c r="L50" s="1"/>
       <c r="M50" s="1"/>
       <c r="N50" s="1"/>
@@ -7004,22 +7250,22 @@
     </row>
     <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="B52" s="28" t="s">
+      <c r="B52" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C52" s="28"/>
-      <c r="D52" s="28" t="s">
+      <c r="C52" s="29"/>
+      <c r="D52" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28" t="s">
+      <c r="E52" s="29"/>
+      <c r="F52" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G52" s="28"/>
-      <c r="H52" s="28" t="s">
+      <c r="G52" s="29"/>
+      <c r="H52" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="I52" s="28"/>
+      <c r="I52" s="29"/>
       <c r="J52" s="1" t="s">
         <v>5</v>
       </c>
@@ -7157,18 +7403,18 @@
     </row>
     <row r="57" spans="1:27" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
-      <c r="B57" s="26" t="s">
+      <c r="B57" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="C57" s="27"/>
-      <c r="D57" s="27"/>
-      <c r="E57" s="27"/>
-      <c r="F57" s="27"/>
-      <c r="G57" s="27"/>
-      <c r="H57" s="27"/>
-      <c r="I57" s="27"/>
-      <c r="J57" s="27"/>
-      <c r="K57" s="27"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="28"/>
+      <c r="E57" s="28"/>
+      <c r="F57" s="28"/>
+      <c r="G57" s="28"/>
+      <c r="H57" s="28"/>
+      <c r="I57" s="28"/>
+      <c r="J57" s="28"/>
+      <c r="K57" s="28"/>
       <c r="L57" s="1"/>
       <c r="M57" s="1"/>
       <c r="N57" s="1"/>
@@ -7188,22 +7434,22 @@
     </row>
     <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
-      <c r="B58" s="28" t="s">
+      <c r="B58" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="28"/>
-      <c r="D58" s="28" t="s">
+      <c r="C58" s="29"/>
+      <c r="D58" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E58" s="28"/>
-      <c r="F58" s="28" t="s">
+      <c r="E58" s="29"/>
+      <c r="F58" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="G58" s="28"/>
-      <c r="H58" s="28" t="s">
+      <c r="G58" s="29"/>
+      <c r="H58" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="I58" s="28"/>
+      <c r="I58" s="29"/>
       <c r="J58" s="1" t="s">
         <v>5</v>
       </c>
@@ -7373,6 +7619,74 @@
     </row>
   </sheetData>
   <mergeCells count="84">
+    <mergeCell ref="G60:G61"/>
+    <mergeCell ref="H60:H61"/>
+    <mergeCell ref="I60:I61"/>
+    <mergeCell ref="B60:B61"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="D60:D61"/>
+    <mergeCell ref="E60:E61"/>
+    <mergeCell ref="F60:F61"/>
+    <mergeCell ref="B57:K57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="F58:G58"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="H15:H19"/>
+    <mergeCell ref="I15:I19"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="H13:I13"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="I7:I9"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B11:K11"/>
+    <mergeCell ref="B21:K21"/>
+    <mergeCell ref="B15:B19"/>
+    <mergeCell ref="C15:C19"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="E15:E19"/>
+    <mergeCell ref="F15:F19"/>
+    <mergeCell ref="G15:G19"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G25:G33"/>
+    <mergeCell ref="H25:H33"/>
+    <mergeCell ref="I25:I33"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="H23:I23"/>
+    <mergeCell ref="B25:B33"/>
+    <mergeCell ref="C25:C33"/>
+    <mergeCell ref="D25:D33"/>
+    <mergeCell ref="E25:E33"/>
+    <mergeCell ref="F25:F33"/>
+    <mergeCell ref="B35:K35"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="H37:I37"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="F45:G45"/>
+    <mergeCell ref="H45:I45"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="C39:C41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="H39:H41"/>
     <mergeCell ref="G54:G55"/>
     <mergeCell ref="H54:H55"/>
     <mergeCell ref="I54:I55"/>
@@ -7389,74 +7703,6 @@
     <mergeCell ref="F54:F55"/>
     <mergeCell ref="I39:I41"/>
     <mergeCell ref="B43:K43"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="F45:G45"/>
-    <mergeCell ref="H45:I45"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="H39:H41"/>
-    <mergeCell ref="B35:K35"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="H37:I37"/>
-    <mergeCell ref="G25:G33"/>
-    <mergeCell ref="H25:H33"/>
-    <mergeCell ref="I25:I33"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="F23:G23"/>
-    <mergeCell ref="H23:I23"/>
-    <mergeCell ref="B25:B33"/>
-    <mergeCell ref="C25:C33"/>
-    <mergeCell ref="D25:D33"/>
-    <mergeCell ref="E25:E33"/>
-    <mergeCell ref="F25:F33"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B11:K11"/>
-    <mergeCell ref="B21:K21"/>
-    <mergeCell ref="B15:B19"/>
-    <mergeCell ref="C15:C19"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="E15:E19"/>
-    <mergeCell ref="F15:F19"/>
-    <mergeCell ref="G15:G19"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="H15:H19"/>
-    <mergeCell ref="I15:I19"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="H13:I13"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="I7:I9"/>
-    <mergeCell ref="B57:K57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="F58:G58"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="G60:G61"/>
-    <mergeCell ref="H60:H61"/>
-    <mergeCell ref="I60:I61"/>
-    <mergeCell ref="B60:B61"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="D60:D61"/>
-    <mergeCell ref="E60:E61"/>
-    <mergeCell ref="F60:F61"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7466,10 +7712,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="C3:W48"/>
+  <dimension ref="C3:AD48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E47" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M70" sqref="M70"/>
+    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z13" sqref="Z13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7479,7 +7725,7 @@
     <col min="4" max="4" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C3" s="14" t="s">
         <v>0</v>
       </c>
@@ -7490,7 +7736,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C4" s="13" t="s">
         <v>1</v>
       </c>
@@ -7500,7 +7746,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>8</v>
       </c>
@@ -7513,7 +7759,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>66</v>
       </c>
@@ -7523,7 +7769,7 @@
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
     </row>
-    <row r="7" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>74</v>
       </c>
@@ -7533,14 +7779,14 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:30" x14ac:dyDescent="0.25">
       <c r="D8" s="12" t="s">
         <v>65</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C9" s="12"/>
       <c r="D9" s="12" t="s">
         <v>67</v>
@@ -7548,7 +7794,7 @@
       <c r="E9" s="12"/>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C10" s="12"/>
       <c r="D10" s="12" t="s">
         <v>68</v>
@@ -7556,7 +7802,7 @@
       <c r="E10" s="12"/>
       <c r="F10" s="12"/>
     </row>
-    <row r="11" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C11" s="12"/>
       <c r="D11" s="12" t="s">
         <v>69</v>
@@ -7564,7 +7810,7 @@
       <c r="E11" s="12"/>
       <c r="F11" s="12"/>
     </row>
-    <row r="12" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C12" s="12"/>
       <c r="D12" s="12" t="s">
         <v>70</v>
@@ -7577,8 +7823,14 @@
       <c r="V12" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="13" spans="3:22" x14ac:dyDescent="0.25">
+      <c r="Z12" t="s">
+        <v>151</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="13" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C13" s="12"/>
       <c r="D13" s="12" t="s">
         <v>71</v>
@@ -7586,7 +7838,7 @@
       <c r="E13" s="12"/>
       <c r="F13" s="12"/>
     </row>
-    <row r="14" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C14" s="12"/>
       <c r="D14" s="12" t="s">
         <v>72</v>
@@ -7594,7 +7846,7 @@
       <c r="E14" s="12"/>
       <c r="F14" s="12"/>
     </row>
-    <row r="15" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C15" s="12"/>
       <c r="D15" s="12" t="s">
         <v>73</v>
@@ -7602,7 +7854,7 @@
       <c r="E15" s="12"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="3:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="12"/>
@@ -8093,10 +8345,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="C4:AF95"/>
+  <dimension ref="C4:AF111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8264,8 +8516,27 @@
         <v>143</v>
       </c>
     </row>
+    <row r="99" spans="3:8" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="C99" s="33" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="109" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>154</v>
+      </c>
+      <c r="H109" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="111" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C111" t="s">
+        <v>156</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>